<commit_message>
Penambahan fotifikasi sukses dan gagal pada function import
</commit_message>
<xml_diff>
--- a/assets/file_format/format_Employee.xlsx
+++ b/assets/file_format/format_Employee.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>NIP</t>
   </si>
@@ -59,7 +59,7 @@
     <t>RW</t>
   </si>
   <si>
-    <t>DESA</t>
+    <t>KELURAHAN</t>
   </si>
   <si>
     <t>KECAMATAN</t>
@@ -149,73 +149,22 @@
     <t>ID JOB TITLE</t>
   </si>
   <si>
+    <t>Laki-Laki</t>
+  </si>
+  <si>
+    <t>akademik</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Perempuan</t>
+  </si>
+  <si>
     <t>hris</t>
   </si>
   <si>
-    <t>HENDRI ANGGARA</t>
-  </si>
-  <si>
-    <t>ndrianggara</t>
-  </si>
-  <si>
-    <t>Laki-Laki</t>
-  </si>
-  <si>
-    <t>AB</t>
-  </si>
-  <si>
-    <t>SMP PUTRA</t>
-  </si>
-  <si>
-    <t>JL KEMENANGAN V</t>
-  </si>
-  <si>
-    <t>jakarta barat</t>
-  </si>
-  <si>
-    <t>tamansari</t>
-  </si>
-  <si>
-    <t>ndrianggar@gmail.com</t>
-  </si>
-  <si>
-    <t>kuningan</t>
-  </si>
-  <si>
-    <t>32112332323232</t>
-  </si>
-  <si>
-    <t>231321323232321</t>
-  </si>
-  <si>
     <t>Nikah</t>
-  </si>
-  <si>
-    <t>Ruki</t>
-  </si>
-  <si>
-    <t>30,20</t>
-  </si>
-  <si>
-    <t>02197600722</t>
-  </si>
-  <si>
-    <t>Rusmani</t>
-  </si>
-  <si>
-    <t>Rusman</t>
-  </si>
-  <si>
-    <t>321345465233212</t>
-  </si>
-  <si>
-    <t>akademik</t>
-  </si>
-  <si>
-    <t>Single</t>
-  </si>
-  <si>
-    <t>Perempuan</t>
   </si>
   <si>
     <t>Duda/Janda</t>
@@ -227,10 +176,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -266,28 +215,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -308,9 +244,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -340,16 +275,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -364,38 +315,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -416,19 +365,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,157 +533,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,24 +570,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -654,11 +590,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -688,16 +622,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -716,18 +650,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -737,130 +686,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -874,7 +823,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1196,8 +1144,8 @@
   <sheetPr/>
   <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AR2" sqref="AR2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AR2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1379,139 +1327,23 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:44">
-      <c r="A2">
-        <v>201383169</v>
-      </c>
-      <c r="B2">
-        <v>12345</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M2">
-        <v>3</v>
-      </c>
-      <c r="N2">
-        <v>3</v>
-      </c>
-      <c r="O2" t="s">
-        <v>51</v>
-      </c>
-      <c r="P2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q2">
-        <v>11120</v>
-      </c>
-      <c r="R2">
-        <v>323232321</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="T2" t="s">
-        <v>54</v>
-      </c>
-      <c r="U2" s="4">
-        <v>33201</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="X2">
-        <v>1</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z2">
-        <v>2</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB2" s="4">
-        <v>43793</v>
-      </c>
-      <c r="AC2">
-        <v>1</v>
-      </c>
-      <c r="AD2">
-        <v>3</v>
-      </c>
-      <c r="AE2">
-        <v>2019</v>
-      </c>
-      <c r="AF2">
-        <v>30</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH2" s="4">
-        <v>43793</v>
-      </c>
-      <c r="AI2">
-        <v>3</v>
-      </c>
-      <c r="AJ2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO2">
-        <v>4</v>
-      </c>
-      <c r="AP2">
-        <v>46546565564</v>
-      </c>
-      <c r="AQ2">
-        <v>1</v>
-      </c>
-      <c r="AR2">
-        <v>12</v>
-      </c>
+    <row r="2" spans="19:34">
+      <c r="S2" s="3"/>
+      <c r="T2"/>
+      <c r="U2" s="4"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2"/>
+      <c r="AD2"/>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -1525,9 +1357,6 @@
       <formula1>SOURCE!$F$4:$F$6</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" display="ndrianggar@gmail.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
@@ -1549,29 +1378,29 @@
   <sheetData>
     <row r="4" spans="4:6">
       <c r="D4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="4:6">
       <c r="D5" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="6:6">
       <c r="F6" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Aplikasi tgl 27-11-19
</commit_message>
<xml_diff>
--- a/assets/file_format/format_Employee.xlsx
+++ b/assets/file_format/format_Employee.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="8940"/>
+    <workbookView windowWidth="23303" windowHeight="4223"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,8 +14,30 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>it_ih</author>
+  </authors>
+  <commentList>
+    <comment ref="S1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>FORMAT YYYY/MM/DD</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>NIP</t>
   </si>
@@ -26,126 +48,129 @@
     <t>HAK AKSES APLIKASI</t>
   </si>
   <si>
+    <t>NAMA LENGKAP</t>
+  </si>
+  <si>
+    <t>NAMA PANGGILAN</t>
+  </si>
+  <si>
+    <t>NO KTP</t>
+  </si>
+  <si>
+    <t>NO KK</t>
+  </si>
+  <si>
+    <t>AGAMA</t>
+  </si>
+  <si>
+    <t>JENIS KELAMIN</t>
+  </si>
+  <si>
+    <t>ALAMAT</t>
+  </si>
+  <si>
+    <t>ID PROVINSI</t>
+  </si>
+  <si>
+    <t>ID KABUPATEN</t>
+  </si>
+  <si>
+    <t>ID KECAMATAN</t>
+  </si>
+  <si>
+    <t>ID KELURAHAN</t>
+  </si>
+  <si>
+    <t>KODE POS</t>
+  </si>
+  <si>
+    <t>NO TELEPON</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>TEMPAT LAHIR</t>
+  </si>
+  <si>
+    <t>TANGGAL LAHIR</t>
+  </si>
+  <si>
+    <t>ID NEGARA</t>
+  </si>
+  <si>
+    <t>STATUS NIKAH</t>
+  </si>
+  <si>
+    <t>JUMLAH ANAK</t>
+  </si>
+  <si>
+    <t>ID JENJANG PEND</t>
+  </si>
+  <si>
+    <t>ID UNIV</t>
+  </si>
+  <si>
+    <t>ID FAKULTAS</t>
+  </si>
+  <si>
+    <t>TAHUN LULUS</t>
+  </si>
+  <si>
+    <t>ID JURUSAN</t>
+  </si>
+  <si>
+    <t>IPK</t>
+  </si>
+  <si>
+    <t>TGL MULAI BERGABUNG</t>
+  </si>
+  <si>
+    <t>ID STATUS KARYAWAN</t>
+  </si>
+  <si>
+    <t>NOMOR DARURAT</t>
+  </si>
+  <si>
+    <t>NAMA KONTAK DARURAT</t>
+  </si>
+  <si>
+    <t>KEAHLIAN BHS ENG</t>
+  </si>
+  <si>
+    <t>KEAHLIAN BHS ARB</t>
+  </si>
+  <si>
+    <t>SERTIFIKAT BHS ENG</t>
+  </si>
+  <si>
+    <t>SERTIFIKAT BHS ARB</t>
+  </si>
+  <si>
+    <t>TILAWAH AL-QURAN</t>
+  </si>
+  <si>
+    <t>HAFALAN AL-QURAN</t>
+  </si>
+  <si>
+    <t>PELATIHAN YG DIINGINKAN</t>
+  </si>
+  <si>
+    <t>PENGISI KAJIAN</t>
+  </si>
+  <si>
+    <t>AKTIFITAS KAJIAN</t>
+  </si>
+  <si>
+    <t>KEAHLIAN KOMPUTER</t>
+  </si>
+  <si>
+    <t>ID DIVISI</t>
+  </si>
+  <si>
     <t>ID JABATAN</t>
   </si>
   <si>
-    <t>LEVEL</t>
-  </si>
-  <si>
-    <t>NAMA</t>
-  </si>
-  <si>
-    <t>NAMA PANGGILAN</t>
-  </si>
-  <si>
-    <t>AGAMA</t>
-  </si>
-  <si>
-    <t>JENIS KELAMIN</t>
-  </si>
-  <si>
-    <t>GOLONGAN DARAH</t>
-  </si>
-  <si>
-    <t>UNIT</t>
-  </si>
-  <si>
-    <t>ALAMAT</t>
-  </si>
-  <si>
-    <t>RT</t>
-  </si>
-  <si>
-    <t>RW</t>
-  </si>
-  <si>
-    <t>KELURAHAN</t>
-  </si>
-  <si>
-    <t>KECAMATAN</t>
-  </si>
-  <si>
-    <t>KODE POS</t>
-  </si>
-  <si>
-    <t>NO TELP</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>TEMPAT LAHIR</t>
-  </si>
-  <si>
-    <t>TANGGAL LAHIR</t>
-  </si>
-  <si>
-    <t>NO KTP</t>
-  </si>
-  <si>
-    <t>NPWP</t>
-  </si>
-  <si>
-    <t>ID NEGARA</t>
-  </si>
-  <si>
-    <t>STATUS NIKAH</t>
-  </si>
-  <si>
-    <t>JUMLAH ANAK</t>
-  </si>
-  <si>
-    <t>NAMA IBU</t>
-  </si>
-  <si>
-    <t>MULAI TUGAS</t>
-  </si>
-  <si>
-    <t>ID JENJANG PENDIDIKAN</t>
-  </si>
-  <si>
-    <t>ID UNIVERSITAS</t>
-  </si>
-  <si>
-    <t>TAHUN LULUS</t>
-  </si>
-  <si>
-    <t>ID JURUSAN UNIVERSITAS</t>
-  </si>
-  <si>
-    <t>IPK</t>
-  </si>
-  <si>
-    <t>TGL BERGABUNG</t>
-  </si>
-  <si>
-    <t>ID STATUS PEGAWAI</t>
-  </si>
-  <si>
-    <t>NOMOR DARURAT 1</t>
-  </si>
-  <si>
-    <t>NAMA ORANG DARURAT 1</t>
-  </si>
-  <si>
-    <t>NOMOR DARURAT 2</t>
-  </si>
-  <si>
-    <t>NAMA ORANG DARURAT 2</t>
-  </si>
-  <si>
-    <t>RELASI KK</t>
-  </si>
-  <si>
-    <t>ID DIVISI</t>
-  </si>
-  <si>
-    <t>NO KK</t>
-  </si>
-  <si>
-    <t>ID CABANG</t>
-  </si>
-  <si>
     <t>ID JOB TITLE</t>
   </si>
   <si>
@@ -165,6 +190,9 @@
   </si>
   <si>
     <t>Nikah</t>
+  </si>
+  <si>
+    <t>akademik, hris</t>
   </si>
   <si>
     <t>Duda/Janda</t>
@@ -177,11 +205,11 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,7 +243,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -223,7 +251,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,17 +280,49 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -267,40 +334,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -315,39 +350,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
     </font>
   </fonts>
   <fills count="33">
@@ -365,19 +398,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,7 +536,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,145 +566,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,54 +601,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -636,6 +631,39 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -651,24 +679,29 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -686,130 +719,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1142,10 +1175,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AR2"/>
+  <dimension ref="A1:AS2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AR2"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AS2" sqref="AS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1153,8 +1186,8 @@
     <col min="1" max="1" width="10.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="11.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="20.2222222222222" customWidth="1"/>
-    <col min="4" max="4" width="11.8888888888889" customWidth="1"/>
-    <col min="5" max="5" width="6.66666666666667" customWidth="1"/>
+    <col min="4" max="4" width="16.2222222222222" customWidth="1"/>
+    <col min="5" max="5" width="18.7777777777778" customWidth="1"/>
     <col min="6" max="6" width="17.6666666666667" customWidth="1"/>
     <col min="7" max="7" width="18.7777777777778" customWidth="1"/>
     <col min="8" max="8" width="8.33333333333333" customWidth="1"/>
@@ -1162,8 +1195,8 @@
     <col min="10" max="10" width="19" customWidth="1"/>
     <col min="11" max="11" width="5.88888888888889" customWidth="1"/>
     <col min="12" max="12" width="18.2222222222222" customWidth="1"/>
-    <col min="13" max="13" width="3.77777777777778" customWidth="1"/>
-    <col min="14" max="14" width="4.55555555555556" customWidth="1"/>
+    <col min="13" max="13" width="15.5555555555556" customWidth="1"/>
+    <col min="14" max="14" width="14.8888888888889" customWidth="1"/>
     <col min="15" max="15" width="12.4444444444444" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
     <col min="17" max="17" width="10.2222222222222" customWidth="1"/>
@@ -1178,10 +1211,10 @@
     <col min="27" max="27" width="10.7777777777778" customWidth="1"/>
     <col min="28" max="28" width="14.1111111111111" customWidth="1"/>
     <col min="29" max="29" width="24" customWidth="1"/>
-    <col min="30" max="30" width="15.8888888888889" customWidth="1"/>
-    <col min="31" max="31" width="14.1111111111111" customWidth="1"/>
+    <col min="30" max="30" width="22.2222222222222" customWidth="1"/>
+    <col min="31" max="31" width="18.1111111111111" customWidth="1"/>
     <col min="32" max="32" width="25.4444444444444" customWidth="1"/>
-    <col min="33" max="33" width="6.11111111111111" customWidth="1"/>
+    <col min="33" max="33" width="19.2222222222222" customWidth="1"/>
     <col min="34" max="34" width="16.6666666666667" customWidth="1"/>
     <col min="35" max="35" width="20.1111111111111" customWidth="1"/>
     <col min="36" max="36" width="19.7777777777778" customWidth="1"/>
@@ -1190,10 +1223,11 @@
     <col min="41" max="41" width="9" customWidth="1"/>
     <col min="42" max="42" width="12.8888888888889" customWidth="1"/>
     <col min="43" max="43" width="11.2222222222222" customWidth="1"/>
-    <col min="44" max="44" width="12.1111111111111" customWidth="1"/>
+    <col min="44" max="44" width="11.8888888888889" customWidth="1"/>
+    <col min="45" max="45" width="13.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:44">
+    <row r="1" s="1" customFormat="1" spans="1:45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1325,40 +1359,32 @@
       </c>
       <c r="AR1" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="19:34">
       <c r="S2" s="3"/>
-      <c r="T2"/>
       <c r="U2" s="4"/>
-      <c r="V2"/>
-      <c r="W2"/>
-      <c r="X2"/>
-      <c r="Y2"/>
-      <c r="Z2"/>
-      <c r="AA2"/>
       <c r="AB2" s="4"/>
-      <c r="AC2"/>
-      <c r="AD2"/>
-      <c r="AE2"/>
-      <c r="AF2"/>
-      <c r="AG2"/>
       <c r="AH2" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
-      <formula1>SOURCE!$E$4:$E$5</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
       <formula1>SOURCE!$D$4:$D$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2">
       <formula1>SOURCE!$F$4:$F$6</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+      <formula1>SOURCE!$E$4:$E$32</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1368,39 +1394,43 @@
   <dimension ref="D4:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="5"/>
   <cols>
     <col min="4" max="4" width="12.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="13.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="4:6">
       <c r="D4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="4:6">
       <c r="D5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="6" spans="6:6">
+    <row r="6" spans="5:6">
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>